<commit_message>
Changes due to ecuacion-modules update.
</commit_message>
<xml_diff>
--- a/ecuacion-tool-housekeep-db/local-test/housekeep-db(fmt-v1.3.0-en)_sample.xlsx
+++ b/ecuacion-tool-housekeep-db/local-test/housekeep-db(fmt-v1.3.0-en)_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yosuke.tanaka/Desktop/development/git/ecuacion-tools/ecuacion-tool-housekeep-db/local-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F63972-FCCE-B24A-AA98-776036335165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07765D3D-4BCD-8243-8971-A6BFD76BB4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="27580" windowHeight="9760" activeTab="4" xr2:uid="{8AED4C0F-E98F-E547-A0B0-59373B747A30}"/>
   </bookViews>
@@ -626,16 +626,16 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2284,21 +2284,21 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="26"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -2391,7 +2391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789F72C4-22B4-0242-AA9D-05DCD1C7C1AF}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -2426,33 +2426,33 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="23" t="s">
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
       <c r="K4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -2531,7 +2531,7 @@
         <v>11</v>
       </c>
       <c r="J6" s="8">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="K6" s="8"/>
       <c r="N6" s="8"/>
@@ -2566,7 +2566,7 @@
         <v>11</v>
       </c>
       <c r="J7" s="8">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="N7" s="8"/>
     </row>
@@ -2734,19 +2734,19 @@
       <c r="D4" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="23" t="s">
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -3009,12 +3009,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">

</xml_diff>